<commit_message>
Updated test form to include parameters
</commit_message>
<xml_diff>
--- a/extras/test-form/Ranking choices.xlsx
+++ b/extras/test-form/Ranking choices.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3622" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10510" uniqueCount="426">
   <si>
     <t>deviceid</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2806,6 +2806,15 @@
   </si>
   <si>
     <t>randomized custom-rankingchoices</t>
+  </si>
+  <si>
+    <t>Bananas&lt;br&gt;Bananas!</t>
+  </si>
+  <si>
+    <t>randomized custom-rankingchoices(allowdef=1, numbers=0)</t>
+  </si>
+  <si>
+    <t>randomized custom-rankingchoices(allowdef=0, numbers=1)</t>
   </si>
 </sst>
 </file>
@@ -6560,7 +6569,7 @@
         <v>407</v>
       </c>
       <c r="F11" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="I11" s="11" t="s">
         <v>380</v>
@@ -6887,7 +6896,7 @@
         <v>399</v>
       </c>
       <c r="C5" t="s">
-        <v>400</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -6998,7 +7007,7 @@
       </c>
       <c r="C2" s="17" t="str">
         <f>TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2003301905</v>
+        <v>2004132036</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>380</v>

</xml_diff>